<commit_message>
Updated notebook4 images to embed fonts, save new size for publication
</commit_message>
<xml_diff>
--- a/CSVs/Table3.xlsx
+++ b/CSVs/Table3.xlsx
@@ -456,10 +456,10 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>4.378008515635884</v>
+        <v>4.378008515632246</v>
       </c>
       <c r="D2">
-        <v>0.1120282443460937</v>
+        <v>0.1120282443462975</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -474,10 +474,10 @@
         <v>0.0004022495850327625</v>
       </c>
       <c r="I2">
-        <v>1219.539467950043</v>
+        <v>1219.539467952261</v>
       </c>
       <c r="J2">
-        <v>0.0008199816621604935</v>
+        <v>0.000819981662159002</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -498,10 +498,10 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>0.0007026537434599023</v>
+        <v>0.0007026537434601243</v>
       </c>
       <c r="H3">
-        <v>0.0008013544428964036</v>
+        <v>0.000801354442896657</v>
       </c>
       <c r="I3">
         <v>139.1019803881618</v>
@@ -528,10 +528,10 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <v>0.0007487348573980146</v>
+        <v>0.0007487348573982366</v>
       </c>
       <c r="H4">
-        <v>0.0007921986271113865</v>
+        <v>0.0007921986271116217</v>
       </c>
       <c r="I4">
         <v>146.2039793486119</v>
@@ -558,10 +558,10 @@
         <v>2</v>
       </c>
       <c r="G5">
-        <v>0.001453990146817019</v>
+        <v>0.00145399014681713</v>
       </c>
       <c r="H5">
-        <v>0.001951960488082428</v>
+        <v>0.001951960488082577</v>
       </c>
       <c r="I5">
         <v>0.2674206882717506</v>
@@ -620,10 +620,10 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0.0007024110033577724</v>
+        <v>0.0007024110033579944</v>
       </c>
       <c r="H7">
-        <v>0.0008010776054624306</v>
+        <v>0.0008010776054626841</v>
       </c>
       <c r="I7">
         <v>1.335220619580411</v>
@@ -650,10 +650,10 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>0.0007319420574249946</v>
+        <v>0.0007319420574248836</v>
       </c>
       <c r="H8">
-        <v>0.0007744310115762776</v>
+        <v>0.0007744310115761603</v>
       </c>
       <c r="I8">
         <v>1.543449401768253</v>
@@ -742,10 +742,10 @@
         <v>4</v>
       </c>
       <c r="G11">
-        <v>0.0009289143052800819</v>
+        <v>0.000928914305280526</v>
       </c>
       <c r="H11">
-        <v>0.00105939748067207</v>
+        <v>0.001059397480672577</v>
       </c>
       <c r="I11">
         <v>372211.4691854921</v>
@@ -772,10 +772,10 @@
         <v>4</v>
       </c>
       <c r="G12">
-        <v>0.0007570447009103143</v>
+        <v>0.0007570447009104253</v>
       </c>
       <c r="H12">
-        <v>0.0008009908538347844</v>
+        <v>0.000800990853834902</v>
       </c>
       <c r="I12">
         <v>1517261.473911633</v>
@@ -805,7 +805,7 @@
         <v>0.001756157484139598</v>
       </c>
       <c r="H13">
-        <v>0.002357615715206175</v>
+        <v>0.002357615715206176</v>
       </c>
       <c r="I13">
         <v>321.5222219275826</v>

</xml_diff>